<commit_message>
work on the pahrmacy price
</commit_message>
<xml_diff>
--- a/files/product_price_list.xlsx
+++ b/files/product_price_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aquacy\Documents\last\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3276174D-40B1-41C2-9896-95EA701DBEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A813D2F0-3E28-4096-93AF-BB517486B3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4917,12 +4917,14 @@
   <dimension ref="A1:Y1224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>